<commit_message>
Add updated Excel file
</commit_message>
<xml_diff>
--- a/data/raw/sources_links_to_raw_data.xlsx
+++ b/data/raw/sources_links_to_raw_data.xlsx
@@ -2,21 +2,29 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitaetstgallen-my.sharepoint.com/personal/matthiaskonstantin_wehmeyer_student_unisg_ch/Documents/02_2nd Semester/02_NLP/01_Project/clin_IQ/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/367d389d4ff35ead/Dokumente/Master/2Semester/NLP/clin_IQ/clin_IQ/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{50353B95-93DE-4443-998C-A8CC9E367E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2712AD5B-33A6-434A-A184-2AE28C62FDE1}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="8_{50353B95-93DE-4443-998C-A8CC9E367E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06238353-1990-45F7-A272-82CEF912117B}"/>
   <bookViews>
-    <workbookView xWindow="-3780" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{DD95ACCF-77B4-4163-8CCF-935C9BBDF4BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DD95ACCF-77B4-4163-8CCF-935C9BBDF4BE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Datasets" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Datasets_Final" sheetId="4" r:id="rId1"/>
+    <sheet name="Dataset_Search" sheetId="2" r:id="rId2"/>
+    <sheet name="Q&amp;A_Data_Formats" sheetId="5" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dataset_Search!$B$5:$H$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Datasets_Final!$B$5:$G$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
   <si>
     <t>Datasets</t>
   </si>
@@ -324,6 +332,119 @@
   </si>
   <si>
     <t>1'270</t>
+  </si>
+  <si>
+    <t>Question Types</t>
+  </si>
+  <si>
+    <t>Short Answer</t>
+  </si>
+  <si>
+    <t>True False</t>
+  </si>
+  <si>
+    <t>Multiple Choice</t>
+  </si>
+  <si>
+    <t>Multi  Hop</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>21,645,374
+Do mitochondria play a role in remodelling lace plant leaves during programmed cell death?
+{ "contexts": [ "Programmed cell death (PCD) is the regulated death of cells within an organism. The lace plant (Aponogeton madagascariensis) produces perforations in its leaves through PCD. The leaves of the plant consist of a latticework of longitudinal and transverse veins enclosing areoles. PCD occurs in the cells at the center of these areoles and progresses outwards, stopping approximately five cells from the vasculature. The role of mitochondria during PCD has been recognized in animals; however, it has been less studied during PCD in plants.", "The following paper elucidates the role of mitochondrial dynamics during developmentally regulated PCD in vivo in A. madagascariensis. A single areole within a window stage leaf (PCD is occurring) was divided into three areas based on the progression of PCD; cells that will not undergo PCD (NPCD), cells in early stages of PCD (EPCD), and cells in late stages of PCD (LPCD). Window stage leaves were stained with the mitochondrial dye MitoTracker Red CMXRos and examined. Mitochondrial dynamics were delineated into four categories (M1-M4) based on characteristics including distribution, motility, and membrane potential (ΔΨm). A TUNEL assay showed fragmented nDNA in a gradient over these mitochondrial stages. Chloroplasts and transvacuolar strands were also examined using live cell imaging. The possible importance of mitochondrial permeability transition pore (PTP) formation during PCD was indirectly examined via in vivo cyclosporine A (CsA) treatment. This treatment resulted in lace plant leaves with a significantly lower number of perforations compared to controls, and that displayed mitochondrial dynamics similar to that of non-PCD cells." ], "labels": [ "BACKGROUND", "RESULTS" ], "meshes": [ "Alismataceae", "Apoptosis", "Cell Differentiation", "Mitochondria", "Plant Leaves" ], "reasoning_required_pred": [ "y", "e", "s" ], "reasoning_free_pred": [ "y", "e", "s" ] }
+Results depicted mitochondrial dynamics in vivo as PCD progresses within the lace plant, and highlight the correlation of this organelle with other organelles during developmental PCD. To the best of our knowledge, this is the first report of mitochondria and chloroplasts moving on transvacuolar strands to form a ring structure surrounding the nucleus during developmental PCD. Also, for the first time, we have shown the feasibility for the use of CsA in a whole plant system. Overall, our findings implicate the mitochondria as playing a critical and early role in developmentally regulated PCD in the lace plant.
+yes</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/datasets/qiaojin/PubMedQA/viewer/pqa_labeled?views%5B%5D=pqa_labeled</t>
+  </si>
+  <si>
+    <t>Example of the Format</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/datasets/openlifescienceai/medmcqa</t>
+  </si>
+  <si>
+    <t>e9ad821a-c438-4965-9f77-760819dfa155
+Chronic urethral obstruction due to benign prismatic hyperplasia can lead to the following change in kidney parenchyma
+Hyperplasia
+Hyperophy
+Atrophy
+Dyplasia
+2c
+single
+Chronic urethral obstruction because of urinary calculi, prostatic hyperophy, tumors, normal pregnancy, tumors, uterine prolapse or functional disorders cause hydronephrosis which by definition is used to describe dilatation of renal pelvis and calculus associated with progressive atrophy of the kidney due to obstruction to the outflow of urine Refer Robbins 7yh/9,1012,9/e. P950
+Anatomy
+Urinary tract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+The mechanism of action of the medication given blocks cell wall synthesis, which of the following was given?
+[ "A 21-year-old sexually active male complains of fever, pain during urination, and inflammation and pain in the right knee.", "A culture of the joint fluid shows a bacteria that does not ferment maltose and has no polysaccharide capsule.", "The physician orders antibiotic therapy for the patient." ]
+3
+{ "A": "Gentamicin", "B": "Ciprofloxacin", "C": "Ceftriaxone", "D": "Trimethoprim" }
+Ceftriaxone
+C
+{ "gender": "Male", "age": "21 years old", "specialties": [ "Internal Medicine", "Urology" ], "subspecialties": [ "Infectious Disease", "General Urology" ], "specialty_prob": [ 0.6, 0.4 ], "subspecialty_prob": [ 0.6, 0.4 ], "gpt_specialty": "Urology" }
+[ "1. Patient is a 21-year-old male.", "2. Patient is sexually active.", "3. Patient complains of fever.", "4. Patient complains of pain during urination.", "5. Patient complains of inflammation and pain in the right knee.", "6. Culture of joint fluid shows a bacteria.", "7. Bacteria does not ferment maltose.", "8. Bacteria has no polysaccharide capsule.", "9. Physician orders antibiotic therapy for the patient." ]
+[ "1. A culture of the joint fluid shows a bacteria.", "2. The </t>
+  </si>
+  <si>
+    <t>https://huggingface.co/datasets/stellalisy/mediQ</t>
+  </si>
+  <si>
+    <t>&lt;s&gt;[INST]Below is an instruction that describes a task, paired with an input that provides further context. Write a response that appropriately completes the request.  # noqa: E501
+### Instruction:
+Answer this question truthfully
+### Input:
+What is the relationship between very low Mg2+ levels, PTH levels, and Ca2+ levels?
+[INST]
+### Response:
+Very low Mg2+ levels correspond to low PTH levels which in turn results in low Ca2+ levels.&lt;/s&gt;</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/datasets/Ajayaadhi/Medical-QA/viewer/default/train?row=0&amp;views%5B%5D=train</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/datasets/FreedomIntelligence/medical-o1-reasoning-SFT/viewer/en/train?row=0&amp;views%5B%5D=en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In a patient with dermatomyositis as indicated by fatigue, muscle weakness, a scaly rash, elevated creatine kinase-MB, anti-Jo-1 antibodies, and perimysial inflammation, which type of cancer is most often associated with this condition?
+Alright, so when I'm thinking about dermatomyositis, I know it's an inflammatory condition with muscle weakness and a telltale skin rash. It's sometimes linked to certain cancers. Now, I remember reading somewhere that when you have dermatomyositis, there's a higher chance of getting some types of cancer. But which one pops up the most? Let's think about that. From what I recall, ovarian cancer often gets mentioned in this context. That's especially true for women with dermatomyositis. So, it seems like a big contender. However, just pointing out ovarian cancer seems a bit simplistic. With diseases like this, there might be more frequently encountered cancers, especially if you consider both men and women. Lung and stomach cancers are quite common and could potentially have strong links too. They seem like they'd show up in some statistics regarding dermatomyositis. But there was that thought about ovarian cancer having a notable association. Maybe I need to dive into some literature and research findings. Hmm. In some studies, what I often find is ovarian cancer being highlighted for women with dermatomyositis, maybe more consistently than others like stomach or colorectal cancer. Gastric cancer seemed an initial possibility for both genders—could it overshadow ovarian cancer just because it's more common overall? Let's switch lanes and think about the most common cancers overall. For women, breast cancer is always high in any list. Maybe it's the same with dermatomyositis? Is breast cancer actually more common here too? It might even show more prevalence than ovarian cancer across different studies, especially since breast cancer is so frequent in the general female population. After digging deeper into research, I start to see breast cancer's name popping up quite a bit with dermatomyositis. I guess considering all demographics, breast cancer may outpace ovarian cancer. So, upon deeper reflection and pulling all this together, it sounds logical that breast cancer might just be the top association after all with dermatomyositis. At least, that's where my thinking leads me.
+In patients with dermatomyositis, ovarian cancer is the most often associated malignancy, particularly in women. While other types of cancer such as breast, lung, and gastric can </t>
+  </si>
+  <si>
+    <t xml:space="preserve">medmcqa
+7,131
+Urogenital Diaphragm is made up of the following, except:
+Colle's fascia. Explanation: Colle's fascia does not contribute to the Urogenital Diaphragm. It is attached posteriorly to the posterior border of the urogenital diaphragm but does not form pa of this diaphragm. Ref: BDC, Volume 2, 4th Edition, Page 332; Grants Method of Anatomy, 11th Edition, Page 244; Gray's Anatomy, 36th Edition, Page 563
+Finding reasoning paths: 1. Urogenital diaphragm -&gt; Pelvic anatomy -&gt; Muscles and fascia -&gt; Deep perineal pouch 2. Urogenital diaphragm -&gt; Components of the perineum -&gt; Muscles and connective tissue 3. Urogenital diaphragm -&gt; Anatomical structures -&gt; Superficial vs. deep fascia Reasoning Process: 1. The urogenital diaphragm is a structure located in the pelvic region, specifically within the perineum. It is important to understand its composition to determine which structures contribute to its formation. 2. The urogenital diaphragm is primarily composed of the deep transverse perineal muscle and the perineal membrane. These structures are located in the deep perineal pouch, which is a part of the pelvic floor. 3. The perineal membrane is a layer of fascia that provides support and is part of the urogenital diaphragm. It is important to distinguish between the deep fascia, which contributes to the diaphragm, and the superficial fascia, which does not. 4. Colle's fascia is a type of superficial fascia found in the perineal region. It is continuous with the superficial fascia of the abdominal wall and is located more superficially than the structures forming the urogenital diaphragm. 5. Since the urogenital diaphragm is composed of deeper structures, such as the deep transverse perineal muscle and the perineal membrane, superficial fascia like Colle's fascia does not contribute to its formation. Conclusion: Colle's fascia, being a type of superficial fascia, does not contribute to the formation of the urogenital diaphragm.
+Answer Choices: A. Deep transverse </t>
+  </si>
+  <si>
+    <t>https://huggingface.co/datasets/UCSC-VLAA/MedReason</t>
+  </si>
+  <si>
+    <t>susceptibility
+	Who is at risk for Lymphocytic Choriomeningitis (LCM)? ?
+	LCMV infections can occur after exposure to fresh urine, droppings, saliva, or nesting materials fro…</t>
+  </si>
+  <si>
+    <t>medqa_4opt_test_0
+A junior orthopaedic surgery resident is completing a carpal tunnel repair with the department chairman as the attending physician. During the procedure, the resident inadvertently cuts a flexor tendon, which is subsequently repaired without complication. The attending advises the resident not to report this complication in the operative report, stating that disclosure may unnecessarily worry the patient. What is the appropriate next action for the resident to take in this situation?
+Tell the attending that he cannot fail to disclose this mistake</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Rows</t>
   </si>
 </sst>
 </file>
@@ -377,7 +498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,13 +516,34 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -411,7 +553,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -422,6 +564,34 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -441,6 +611,1125 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[sources_links_to_raw_data.xlsx]Datasets_Final!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Question</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Distribution</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Datasets_Final!$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Datasets_Final!$B$19:$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Multi  Hop</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Multiple Choice</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Short Answer</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>True False</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Datasets_Final!$C$19:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>19700</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>241293</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66149</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>211000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB09-4D06-B45C-254B71990F0A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:srgbClr val="0070C0"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>826394</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>23611</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2590084</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>137375</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7ACE0D1-5D9C-01CA-EF8D-AABD14824083}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adria Pop" refreshedDate="45781.481680902776" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="9" xr:uid="{FF369119-401D-4810-8215-7301B48B4C2E}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="C5:E14" sheet="Datasets_Final"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Type" numFmtId="0">
+      <sharedItems count="4">
+        <s v="True False"/>
+        <s v="Multiple Choice"/>
+        <s v="Short Answer"/>
+        <s v="Multi  Hop"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Format" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Rows" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1270" maxValue="211000"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="9">
+  <r>
+    <x v="0"/>
+    <s v="JSON"/>
+    <n v="211000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="parquet"/>
+    <n v="193330"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="JSON"/>
+    <n v="2540"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="csv"/>
+    <n v="49900"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="JSON"/>
+    <n v="19700"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="JSON"/>
+    <n v="12723"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="JSON"/>
+    <n v="32700"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="csv"/>
+    <n v="14979"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="JSON"/>
+    <n v="1270"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{291FE9C1-E1B8-437A-9106-3F8247E3803C}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="B18:C23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Rows" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -759,25 +2048,367 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E989C9E0-4A35-4393-90C7-1E7194E19863}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="B3:U23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="49" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="5" width="20.08984375" customWidth="1"/>
+    <col min="6" max="6" width="49.1796875" customWidth="1"/>
+    <col min="7" max="7" width="118" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="15">
+        <v>211000</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="15">
+        <v>193330</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="15">
+        <v>2540</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="15">
+        <v>49900</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B10" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="15">
+        <v>19700</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="15">
+        <v>12723</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="15">
+        <v>32700</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="15">
+        <v>14979</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="22">
+        <v>1270</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F17" s="8"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="12">
+        <v>19700</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="12">
+        <v>241293</v>
+      </c>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="12">
+        <v>66149</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="12">
+        <v>211000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="12">
+        <v>538142</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B5:G5" xr:uid="{E989C9E0-4A35-4393-90C7-1E7194E19863}"/>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId2" xr:uid="{03DC255A-D878-4ADA-A7BD-A3D5AFEB1B5E}"/>
+    <hyperlink ref="G10" r:id="rId3" xr:uid="{13DCDA7E-BEDA-4B90-BF0D-F7558223C3F7}"/>
+    <hyperlink ref="G11" r:id="rId4" xr:uid="{5C1E7514-B3FC-458F-A44A-761A3470E39F}"/>
+    <hyperlink ref="G12" r:id="rId5" xr:uid="{F4977E86-A6FB-439D-B971-859BF087A92C}"/>
+    <hyperlink ref="G13" r:id="rId6" xr:uid="{F0C79C74-D3A1-4895-969E-ECA7883C6F8E}"/>
+    <hyperlink ref="G14" r:id="rId7" xr:uid="{1752EF1F-D5C6-4E9E-837A-3BA3261C5DA0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId8"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1DF141B7-6670-486C-A5BE-B2634B12BC66}">
+          <x14:formula1>
+            <xm:f>'Q&amp;A_Data_Formats'!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C6:C14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A95848A-0CFC-4E76-9D67-7C196B13FC7A}">
   <dimension ref="B3:V29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="71" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="35.21875" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="49.21875" customWidth="1"/>
-    <col min="8" max="8" width="110.88671875" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="52.36328125" customWidth="1"/>
+    <col min="3" max="3" width="45.90625" customWidth="1"/>
+    <col min="4" max="6" width="20.08984375" customWidth="1"/>
+    <col min="7" max="7" width="49.1796875" customWidth="1"/>
+    <col min="8" max="8" width="110.90625" customWidth="1"/>
+    <col min="9" max="9" width="20.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +2433,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -825,7 +2456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -848,7 +2479,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
@@ -871,7 +2502,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -894,7 +2525,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
@@ -917,7 +2548,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
@@ -940,7 +2571,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
         <v>35</v>
       </c>
@@ -963,7 +2594,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
@@ -986,7 +2617,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
         <v>44</v>
       </c>
@@ -1009,7 +2640,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>48</v>
       </c>
@@ -1032,7 +2663,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
@@ -1055,7 +2686,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
         <v>56</v>
       </c>
@@ -1078,7 +2709,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>63</v>
       </c>
@@ -1101,7 +2732,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>68</v>
       </c>
@@ -1124,7 +2755,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>71</v>
       </c>
@@ -1147,7 +2778,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>81</v>
       </c>
@@ -1170,7 +2801,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>74</v>
       </c>
@@ -1193,7 +2824,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>79</v>
       </c>
@@ -1210,10 +2841,10 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I26" s="4"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I29" s="4"/>
     </row>
   </sheetData>
@@ -1234,14 +2865,57 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E271BE78-903D-42A2-BCCC-574A501483F8}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD55958-EE7B-4121-A507-1AA0344D5375}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added pipeline for dataset creation
</commit_message>
<xml_diff>
--- a/data/raw/sources_links_to_raw_data.xlsx
+++ b/data/raw/sources_links_to_raw_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/367d389d4ff35ead/Dokumente/Master/2Semester/NLP/clin_IQ/clin_IQ/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitaetstgallen-my.sharepoint.com/personal/matthiaskonstantin_wehmeyer_student_unisg_ch/Documents/02_2nd Semester/02_NLP/01_Project/clin_IQ/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="247" documentId="8_{50353B95-93DE-4443-998C-A8CC9E367E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06238353-1990-45F7-A272-82CEF912117B}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="8_{50353B95-93DE-4443-998C-A8CC9E367E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8262F323-ADDB-474C-B44B-0771F78CA834}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DD95ACCF-77B4-4163-8CCF-935C9BBDF4BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{DD95ACCF-77B4-4163-8CCF-935C9BBDF4BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets_Final" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="112">
   <si>
     <t>Datasets</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>Sum of Rows</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -562,9 +565,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -593,6 +593,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
@@ -616,7 +619,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -687,7 +690,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -737,7 +740,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -750,6 +753,62 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -784,6 +843,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-99C8-4CF1-A578-A8C8356E23A6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -799,6 +863,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-99C8-4CF1-A578-A8C8356E23A6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -814,6 +883,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-99C8-4CF1-A578-A8C8356E23A6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -829,6 +903,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-99C8-4CF1-A578-A8C8356E23A6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -923,7 +1002,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -957,7 +1036,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1584,10 +1663,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adria Pop" refreshedDate="45781.481680902776" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="9" xr:uid="{FF369119-401D-4810-8215-7301B48B4C2E}">
   <cacheSource type="worksheet">
@@ -1668,7 +1743,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{291FE9C1-E1B8-437A-9106-3F8247E3803C}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{291FE9C1-E1B8-437A-9106-3F8247E3803C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="B18:C23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -1709,12 +1784,60 @@
   <dataFields count="1">
     <dataField name="Sum of Rows" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="5">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -2052,24 +2175,24 @@
   <sheetPr>
     <tabColor theme="3" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="B3:U23"/>
+  <dimension ref="A3:U23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="49" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" customWidth="1"/>
-    <col min="4" max="5" width="20.08984375" customWidth="1"/>
-    <col min="6" max="6" width="49.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="49.21875" customWidth="1"/>
     <col min="7" max="7" width="118" customWidth="1"/>
-    <col min="8" max="8" width="20.08984375" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2093,284 +2216,312 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="14">
+        <v>19700</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="14">
+        <v>193330</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="14">
+        <v>2540</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="14">
+        <v>12723</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="14">
+        <v>32700</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="14">
+        <v>49900</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="14">
+        <v>14979</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="21">
+        <v>1270</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E14" s="14">
         <v>211000</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F14" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="15">
-        <v>193330</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B8" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="15">
-        <v>2540</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="15">
-        <v>49900</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B10" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="15">
-        <v>19700</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="15">
-        <v>12723</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="15">
-        <v>32700</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="15">
-        <v>14979</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B14" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="22">
-        <v>1270</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="F17" s="8"/>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F17" s="7"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B18" s="10" t="s">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="9" t="s">
         <v>108</v>
       </c>
       <c r="C18" t="s">
         <v>110</v>
       </c>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B19" s="11" t="s">
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>19700</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="11" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="11">
         <v>241293</v>
       </c>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B21" s="11" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="11">
         <v>66149</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="11" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <v>211000</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B23" s="11" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <v>538142</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B5:G5" xr:uid="{E989C9E0-4A35-4393-90C7-1E7194E19863}"/>
+  <autoFilter ref="B5:G5" xr:uid="{E989C9E0-4A35-4393-90C7-1E7194E19863}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:G14">
+      <sortCondition ref="C5"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="G7" r:id="rId2" xr:uid="{03DC255A-D878-4ADA-A7BD-A3D5AFEB1B5E}"/>
-    <hyperlink ref="G10" r:id="rId3" xr:uid="{13DCDA7E-BEDA-4B90-BF0D-F7558223C3F7}"/>
-    <hyperlink ref="G11" r:id="rId4" xr:uid="{5C1E7514-B3FC-458F-A44A-761A3470E39F}"/>
-    <hyperlink ref="G12" r:id="rId5" xr:uid="{F4977E86-A6FB-439D-B971-859BF087A92C}"/>
-    <hyperlink ref="G13" r:id="rId6" xr:uid="{F0C79C74-D3A1-4895-969E-ECA7883C6F8E}"/>
-    <hyperlink ref="G14" r:id="rId7" xr:uid="{1752EF1F-D5C6-4E9E-837A-3BA3261C5DA0}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{13DCDA7E-BEDA-4B90-BF0D-F7558223C3F7}"/>
+    <hyperlink ref="G9" r:id="rId4" xr:uid="{5C1E7514-B3FC-458F-A44A-761A3470E39F}"/>
+    <hyperlink ref="G10" r:id="rId5" xr:uid="{F4977E86-A6FB-439D-B971-859BF087A92C}"/>
+    <hyperlink ref="G12" r:id="rId6" xr:uid="{F0C79C74-D3A1-4895-969E-ECA7883C6F8E}"/>
+    <hyperlink ref="G13" r:id="rId7" xr:uid="{1752EF1F-D5C6-4E9E-837A-3BA3261C5DA0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId8"/>
@@ -2397,18 +2548,18 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.453125" customWidth="1"/>
-    <col min="2" max="2" width="52.36328125" customWidth="1"/>
-    <col min="3" max="3" width="45.90625" customWidth="1"/>
-    <col min="4" max="6" width="20.08984375" customWidth="1"/>
-    <col min="7" max="7" width="49.1796875" customWidth="1"/>
-    <col min="8" max="8" width="110.90625" customWidth="1"/>
-    <col min="9" max="9" width="20.08984375" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="49.21875" customWidth="1"/>
+    <col min="8" max="8" width="110.88671875" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2433,7 +2584,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2456,7 +2607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -2479,7 +2630,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
@@ -2502,7 +2653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -2525,7 +2676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
@@ -2548,7 +2699,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
@@ -2571,7 +2722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>35</v>
       </c>
@@ -2594,7 +2745,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
@@ -2617,7 +2768,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>44</v>
       </c>
@@ -2640,7 +2791,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>48</v>
       </c>
@@ -2663,7 +2814,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
@@ -2686,7 +2837,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>56</v>
       </c>
@@ -2709,7 +2860,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>63</v>
       </c>
@@ -2732,7 +2883,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>68</v>
       </c>
@@ -2755,7 +2906,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>71</v>
       </c>
@@ -2778,7 +2929,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>81</v>
       </c>
@@ -2801,7 +2952,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>74</v>
       </c>
@@ -2824,7 +2975,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>79</v>
       </c>
@@ -2834,17 +2985,17 @@
       <c r="D22" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="I26" s="4"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="I29" s="4"/>
     </row>
   </sheetData>
@@ -2873,20 +3024,20 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -2894,7 +3045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -2902,7 +3053,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -2910,7 +3061,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>91</v>
       </c>

</xml_diff>